<commit_message>
changed the name of the zero lecture
</commit_message>
<xml_diff>
--- a/Course TimeSheet.xlsx
+++ b/Course TimeSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sharif University\Fundamental Programming with Python 1401\Course1401\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772A9DFC-9841-4BCD-A770-1653DE8F50B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8619644-FFEC-4A1E-B108-5A7FFE13EE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">هفته </t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>فرجه های امتحان</t>
+  </si>
+  <si>
+    <t>00-Introduction to Computation and Programming</t>
   </si>
 </sst>
 </file>
@@ -113,7 +116,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d;@"/>
+    <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -166,16 +169,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -460,430 +463,433 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="8.7265625" style="1"/>
     <col min="4" max="4" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="43.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>44938</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>45089</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4">
+      <c r="A6" s="6"/>
+      <c r="B6" s="2">
         <v>4</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>45150</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+      <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="4">
+      <c r="A8" s="6"/>
+      <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+      <c r="A9" s="6">
         <v>6</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="2">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4">
+      <c r="A10" s="6"/>
+      <c r="B10" s="2">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+      <c r="A11" s="2">
         <v>7</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="2">
         <v>9</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
+      <c r="A12" s="2">
         <v>8</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
+      <c r="A13" s="6">
         <v>9</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="2">
         <v>11</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4">
+      <c r="A14" s="6"/>
+      <c r="B14" s="2">
         <v>12</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+      <c r="A15" s="6">
         <v>10</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="2">
         <v>13</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="4">
+      <c r="A16" s="6"/>
+      <c r="B16" s="2">
         <v>14</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
+      <c r="A17" s="2">
         <v>11</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="2">
         <v>15</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>45018</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
+      <c r="A18" s="6">
         <v>12</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="2">
         <v>16</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>45171</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
-      <c r="B19" s="4">
+      <c r="A19" s="6"/>
+      <c r="B19" s="2">
         <v>17</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>45232</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
+      <c r="A20" s="6">
         <v>13</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="2">
         <v>18</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="4">
+      <c r="A21" s="6"/>
+      <c r="B21" s="2">
         <v>19</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
+      <c r="A22" s="6">
         <v>14</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="2">
         <v>20</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="4">
+      <c r="A23" s="6"/>
+      <c r="B23" s="2">
         <v>21</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
+      <c r="A24" s="6">
         <v>15</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="2">
         <v>22</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="4">
+      <c r="A25" s="6"/>
+      <c r="B25" s="2">
         <v>23</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>44929</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="2">
+      <c r="A26" s="6">
         <v>16</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="2">
         <v>24</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>45080</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="4">
+      <c r="A27" s="6"/>
+      <c r="B27" s="2">
         <v>25</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <v>45141</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="4">
+      <c r="A28" s="2">
         <v>17</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="2">
         <v>26</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="4">
+      <c r="A29" s="2">
         <v>18</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="2">
         <v>27</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B30" s="4"/>
+      <c r="B30" s="2"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated title of lectures and added time for ex
</commit_message>
<xml_diff>
--- a/Course TimeSheet.xlsx
+++ b/Course TimeSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sharif University\Fundamental Programming with Python 1401\Course1401\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A9DCDE-66D1-4754-91C9-D8830AB8A3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF5C48E-B0C9-46D4-A78F-34700BD98C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t xml:space="preserve">هفته </t>
   </si>
@@ -114,7 +114,97 @@
     <t>00-Introduction to Programming Applications with Python</t>
   </si>
   <si>
-    <t>02- Introduction to Programming</t>
+    <t>کارگاه</t>
+  </si>
+  <si>
+    <t>05- Control and Loop Structures</t>
+  </si>
+  <si>
+    <t>03- How We Can Represent a Problem?</t>
+  </si>
+  <si>
+    <t>04- Introduction to Objects in Python</t>
+  </si>
+  <si>
+    <t>06- Control and Loop Structures</t>
+  </si>
+  <si>
+    <t>08- The Most Important Data Structures in Python?</t>
+  </si>
+  <si>
+    <t>09- The Most Important Data Structures in Python?</t>
+  </si>
+  <si>
+    <t>14- Exceptions Handling</t>
+  </si>
+  <si>
+    <t>15- What is Object-oriented Programming?</t>
+  </si>
+  <si>
+    <t>16- What is Object-oriented Programming?</t>
+  </si>
+  <si>
+    <t>17- How We Can Evaluate Our Code?</t>
+  </si>
+  <si>
+    <t>18- What are Modules, Packages, and Libraries?</t>
+  </si>
+  <si>
+    <t>19- Visualization for Presentation and better Understanding!</t>
+  </si>
+  <si>
+    <t>20- Simple Text Processing in Python!</t>
+  </si>
+  <si>
+    <t>21- What is Numerical Calculation?</t>
+  </si>
+  <si>
+    <t>22- We Can Read and Analyse any Data with Python</t>
+  </si>
+  <si>
+    <t>23- We Can Read and Analyse any Data with Python</t>
+  </si>
+  <si>
+    <t>مهمان</t>
+  </si>
+  <si>
+    <t>Review!</t>
+  </si>
+  <si>
+    <t>10- Different General Methods in Algorithms Design</t>
+  </si>
+  <si>
+    <t>11- Different General Methods in Algorithms Design</t>
+  </si>
+  <si>
+    <t>12- Different General Methods in Algorithms Design</t>
+  </si>
+  <si>
+    <t>13- Different General Methods in Algorithms Design</t>
+  </si>
+  <si>
+    <t>گیت و گیت هاب (2)</t>
+  </si>
+  <si>
+    <t>سایکیت لرن (1)</t>
+  </si>
+  <si>
+    <t>دسک (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">پروژه </t>
+  </si>
+  <si>
+    <t>07- What is Function?</t>
+  </si>
+  <si>
+    <t>واسط گرافیکی (1)</t>
+  </si>
+  <si>
+    <t>داکر (1)</t>
+  </si>
+  <si>
+    <t>02- Introduction to Programming with Python</t>
   </si>
 </sst>
 </file>
@@ -467,21 +557,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="8.7265625" style="1"/>
     <col min="4" max="4" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="51.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="1"/>
+    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -500,8 +592,14 @@
       <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -517,7 +615,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -533,7 +631,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -545,11 +643,11 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -560,10 +658,12 @@
         <v>45089</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
       <c r="B6" s="2">
         <v>4</v>
@@ -572,10 +672,15 @@
         <v>45150</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -586,10 +691,12 @@
         <v>7</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="2">
         <v>6</v>
@@ -598,10 +705,12 @@
         <v>8</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -612,10 +721,14 @@
         <v>9</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
       <c r="B10" s="2">
         <v>8</v>
@@ -624,10 +737,12 @@
         <v>10</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>7</v>
       </c>
@@ -638,10 +753,12 @@
         <v>11</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -654,10 +771,12 @@
       <c r="D12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>9</v>
       </c>
@@ -668,10 +787,15 @@
         <v>13</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="6"/>
       <c r="B14" s="2">
         <v>12</v>
@@ -680,10 +804,14 @@
         <v>14</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>10</v>
       </c>
@@ -694,10 +822,15 @@
         <v>15</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="2"/>
+      <c r="E15" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="2">
         <v>14</v>
@@ -706,10 +839,12 @@
         <v>16</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>11</v>
       </c>
@@ -720,10 +855,12 @@
         <v>45018</v>
       </c>
       <c r="D17" s="4"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>12</v>
       </c>
@@ -734,10 +871,12 @@
         <v>45171</v>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
       <c r="B19" s="2">
         <v>17</v>
@@ -746,10 +885,12 @@
         <v>45232</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>13</v>
       </c>
@@ -760,10 +901,20 @@
         <v>17</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="2">
+        <v>3</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="2">
         <v>19</v>
@@ -772,10 +923,12 @@
         <v>18</v>
       </c>
       <c r="D21" s="4"/>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>14</v>
       </c>
@@ -786,10 +939,12 @@
         <v>19</v>
       </c>
       <c r="D22" s="4"/>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
       <c r="B23" s="2">
         <v>21</v>
@@ -798,10 +953,12 @@
         <v>20</v>
       </c>
       <c r="D23" s="4"/>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>15</v>
       </c>
@@ -812,10 +969,15 @@
         <v>21</v>
       </c>
       <c r="D24" s="4"/>
-      <c r="E24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
       <c r="B25" s="2">
         <v>23</v>
@@ -824,10 +986,14 @@
         <v>44929</v>
       </c>
       <c r="D25" s="4"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>16</v>
       </c>
@@ -838,10 +1004,12 @@
         <v>45080</v>
       </c>
       <c r="D26" s="4"/>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" s="2">
         <v>25</v>
@@ -850,10 +1018,12 @@
         <v>45141</v>
       </c>
       <c r="D27" s="4"/>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>17</v>
       </c>
@@ -864,10 +1034,12 @@
         <v>22</v>
       </c>
       <c r="D28" s="4"/>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>18</v>
       </c>
@@ -880,10 +1052,17 @@
       <c r="D29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E29" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="2">
+        <v>5</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
updated for Parsa workshop :)
</commit_message>
<xml_diff>
--- a/Course TimeSheet.xlsx
+++ b/Course TimeSheet.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sharif University\Fundamental Programming with Python 1401\Course1401\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF5C48E-B0C9-46D4-A78F-34700BD98C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D71743-7F42-4009-836A-F277BF8D9EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -201,10 +210,10 @@
     <t>واسط گرافیکی (1)</t>
   </si>
   <si>
-    <t>داکر (1)</t>
-  </si>
-  <si>
     <t>02- Introduction to Programming with Python</t>
+  </si>
+  <si>
+    <t>نحوه ذخیره سازی مقادیر در کامپیوتر (1)</t>
   </si>
 </sst>
 </file>
@@ -559,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -569,7 +578,7 @@
     <col min="4" max="4" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="51.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7265625" style="1"/>
-    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
@@ -643,7 +652,7 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -676,9 +685,6 @@
         <v>32</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="1" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
@@ -695,6 +701,9 @@
         <v>30</v>
       </c>
       <c r="F7" s="2"/>
+      <c r="G7" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
@@ -741,6 +750,9 @@
         <v>34</v>
       </c>
       <c r="F10" s="2"/>
+      <c r="G10" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
@@ -791,9 +803,6 @@
         <v>49</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="1" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="6"/>
@@ -908,7 +917,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H20" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
added some update for type of our class
</commit_message>
<xml_diff>
--- a/Course TimeSheet.xlsx
+++ b/Course TimeSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sharif University\Fundamental Programming with Python 1401\Course1401\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C034D8B-373E-4C89-B5B4-B77C58896D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9078867C-9ADA-448F-8C47-77204323C499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t xml:space="preserve">هفته </t>
   </si>
@@ -105,18 +105,9 @@
     <t>13/3</t>
   </si>
   <si>
-    <t>20/3</t>
-  </si>
-  <si>
     <t>توضیحات</t>
   </si>
   <si>
-    <t>نگردیم؟:)</t>
-  </si>
-  <si>
-    <t>فرجه های امتحان</t>
-  </si>
-  <si>
     <t>01- Introduction to Computer System</t>
   </si>
   <si>
@@ -168,9 +159,6 @@
     <t>23- We Can Read and Analyse any Data with Python</t>
   </si>
   <si>
-    <t>مهمان</t>
-  </si>
-  <si>
     <t>Review!</t>
   </si>
   <si>
@@ -214,6 +202,30 @@
   </si>
   <si>
     <t>09- The Most Important Data Structures in Python</t>
+  </si>
+  <si>
+    <t>مهمان (سینا)</t>
+  </si>
+  <si>
+    <t>مهمان (مسعود)</t>
+  </si>
+  <si>
+    <t>17/3</t>
+  </si>
+  <si>
+    <t>کلاس جبرانی</t>
+  </si>
+  <si>
+    <t>مجازی برگزار میشود</t>
+  </si>
+  <si>
+    <t>هیبریدی برگزار میشود</t>
+  </si>
+  <si>
+    <t>قراره که درباره این تاریخ هم با دانشکده مشورت و صحبت کنم</t>
+  </si>
+  <si>
+    <t>!گردش فناورانه</t>
   </si>
 </sst>
 </file>
@@ -568,14 +580,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="8.7265625" style="1"/>
-    <col min="4" max="4" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="51.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7265625" style="1"/>
     <col min="7" max="7" width="27.453125" style="1" bestFit="1" customWidth="1"/>
@@ -593,7 +605,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>3</v>
@@ -602,10 +614,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -620,7 +632,7 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -636,7 +648,7 @@
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -652,7 +664,7 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -668,7 +680,7 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -682,7 +694,7 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -698,11 +710,11 @@
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -715,7 +727,7 @@
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -729,9 +741,11 @@
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="E9" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
@@ -745,13 +759,15 @@
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -764,9 +780,11 @@
       <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="E11" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -781,10 +799,10 @@
         <v>12</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -800,7 +818,7 @@
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -814,7 +832,7 @@
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F14" s="2">
         <v>2</v>
@@ -832,7 +850,7 @@
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F15" s="2"/>
       <c r="H15" s="1">
@@ -849,7 +867,7 @@
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F16" s="2"/>
     </row>
@@ -865,7 +883,7 @@
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -881,7 +899,7 @@
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -895,7 +913,7 @@
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -911,13 +929,13 @@
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F20" s="2">
         <v>3</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H20" s="1">
         <v>1</v>
@@ -933,7 +951,7 @@
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -949,7 +967,7 @@
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -963,7 +981,7 @@
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -979,11 +997,11 @@
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -996,7 +1014,7 @@
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F25" s="2">
         <v>4</v>
@@ -1014,7 +1032,7 @@
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="F26" s="2"/>
     </row>
@@ -1028,7 +1046,7 @@
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F27" s="2"/>
     </row>
@@ -1044,7 +1062,7 @@
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="2" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="F28" s="2"/>
     </row>
@@ -1056,19 +1074,19 @@
         <v>27</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F29" s="2">
         <v>5</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1078,16 +1096,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>